<commit_message>
Changed method to compute qoq CIs
</commit_message>
<xml_diff>
--- a/Data/quarter_on_quarter_Q4.xlsx
+++ b/Data/quarter_on_quarter_Q4.xlsx
@@ -549,10 +549,10 @@
         <v>4.496759984042153</v>
       </c>
       <c r="C2">
-        <v>4.198888601901318</v>
+        <v>0.5473019062485873</v>
       </c>
       <c r="D2">
-        <v>4.080509354437067</v>
+        <v>8.288602944482349</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -563,10 +563,10 @@
         <v>5.426545557333395</v>
       </c>
       <c r="C3">
-        <v>5.8678996256323</v>
+        <v>2.336538197474081</v>
       </c>
       <c r="D3">
-        <v>5.718800444870986</v>
+        <v>8.420925159145698</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -577,10 +577,10 @@
         <v>-2.780077351736532</v>
       </c>
       <c r="C4">
-        <v>-3.232364456083447</v>
+        <v>-5.831459815107165</v>
       </c>
       <c r="D4">
-        <v>-1.581543889725101</v>
+        <v>0.6234400863243339</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -591,10 +591,10 @@
         <v>-2.949046909389508</v>
       </c>
       <c r="C5">
-        <v>-3.464495453779626</v>
+        <v>-5.636901255877069</v>
       </c>
       <c r="D5">
-        <v>-1.941657786589324</v>
+        <v>0.4363987909712375</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -605,10 +605,10 @@
         <v>4.226073429543509</v>
       </c>
       <c r="C6">
-        <v>4.213347523941202</v>
+        <v>1.860057215531952</v>
       </c>
       <c r="D6">
-        <v>4.428431365702767</v>
+        <v>6.55452694385259</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -619,10 +619,10 @@
         <v>0.4626164446735137</v>
       </c>
       <c r="C7">
-        <v>-0.2550681124524834</v>
+        <v>-3.469059361761806</v>
       </c>
       <c r="D7">
-        <v>0.3411018604793536</v>
+        <v>4.044228171379527</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -633,10 +633,10 @@
         <v>-0.3815690553422679</v>
       </c>
       <c r="C8">
-        <v>-0.7688033049375376</v>
+        <v>-2.501748859922448</v>
       </c>
       <c r="D8">
-        <v>-0.1681006807354612</v>
+        <v>1.715977296859039</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -647,10 +647,10 @@
         <v>3.398051521202716</v>
       </c>
       <c r="C9">
-        <v>4.140290053979379</v>
+        <v>-1.026487832326983</v>
       </c>
       <c r="D9">
-        <v>0.6899324444026522</v>
+        <v>8.07446689491873</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -661,10 +661,10 @@
         <v>1.850105436886285</v>
       </c>
       <c r="C10">
-        <v>1.813919739413938</v>
+        <v>-1.891620692598783</v>
       </c>
       <c r="D10">
-        <v>1.873705548530924</v>
+        <v>4.678778177908094</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -675,10 +675,10 @@
         <v>7.49210004187546</v>
       </c>
       <c r="C11">
-        <v>7.727302950195303</v>
+        <v>4.697622100979482</v>
       </c>
       <c r="D11">
-        <v>6.737770965213863</v>
+        <v>10.23117127235673</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -689,10 +689,10 @@
         <v>-2.079651028340723</v>
       </c>
       <c r="C12">
-        <v>-3.262846766632843</v>
+        <v>-5.868388739426789</v>
       </c>
       <c r="D12">
-        <v>-0.8419239397314593</v>
+        <v>2.149573713386155</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -703,10 +703,10 @@
         <v>-0.6496777464566228</v>
       </c>
       <c r="C13">
-        <v>-0.5944779969514036</v>
+        <v>-3.397858862689174</v>
       </c>
       <c r="D13">
-        <v>-0.6409738073367199</v>
+        <v>2.202899183221585</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -717,10 +717,10 @@
         <v>3.643602269412538</v>
       </c>
       <c r="C14">
-        <v>2.839699003307206</v>
+        <v>-2.247565637251847</v>
       </c>
       <c r="D14">
-        <v>4.180768414358527</v>
+        <v>9.582552649439414</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -731,10 +731,10 @@
         <v>1.06128986154348</v>
       </c>
       <c r="C15">
-        <v>0.5605049520288397</v>
+        <v>-2.093849368727063</v>
       </c>
       <c r="D15">
-        <v>1.918284240060375</v>
+        <v>4.486396289097594</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -745,10 +745,10 @@
         <v>-5.46442665787239</v>
       </c>
       <c r="C16">
-        <v>-6.354816633386962</v>
+        <v>-8.206427647871639</v>
       </c>
       <c r="D16">
-        <v>-4.487063538308222</v>
+        <v>-2.388814416703777</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -759,10 +759,10 @@
         <v>-3.256107553236354</v>
       </c>
       <c r="C17">
-        <v>-3.72125905758488</v>
+        <v>-5.781331925614486</v>
       </c>
       <c r="D17">
-        <v>-2.300841858824976</v>
+        <v>-0.6737226720217704</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -773,10 +773,10 @@
         <v>0.1482496280591494</v>
       </c>
       <c r="C18">
-        <v>-0.1932210871175899</v>
+        <v>-4.875271439088824</v>
       </c>
       <c r="D18">
-        <v>-0.2559361793069037</v>
+        <v>5.673794054999504</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -784,13 +784,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>-3.233103716856367</v>
+        <v>-3.233103716856356</v>
       </c>
       <c r="C19">
-        <v>-4.390721782802565</v>
+        <v>-6.79272002661514</v>
       </c>
       <c r="D19">
-        <v>-2.164586775203958</v>
+        <v>0.354039452534427</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -801,10 +801,10 @@
         <v>5.088251026635171</v>
       </c>
       <c r="C20">
-        <v>3.937951978056908</v>
+        <v>-7.029876087379394</v>
       </c>
       <c r="D20">
-        <v>5.993436346852987</v>
+        <v>16.61525665687831</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -815,10 +815,10 @@
         <v>8.577247308000956</v>
       </c>
       <c r="C21">
-        <v>9.034587215340384</v>
+        <v>5.172767133968859</v>
       </c>
       <c r="D21">
-        <v>5.647814649250127</v>
+        <v>12.28708311906699</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -829,10 +829,10 @@
         <v>1.736634908867773</v>
       </c>
       <c r="C22">
-        <v>1.717826412415357</v>
+        <v>-3.629395256345935</v>
       </c>
       <c r="D22">
-        <v>2.412173907094406</v>
+        <v>5.193432380973029</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -843,10 +843,10 @@
         <v>2.873936502380925</v>
       </c>
       <c r="C23">
-        <v>3.91757454039674</v>
+        <v>-5.715341457707702</v>
       </c>
       <c r="D23">
-        <v>2.212680103491538</v>
+        <v>8.646068047429578</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -854,13 +854,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>2.889754734408889</v>
+        <v>2.889754734408911</v>
       </c>
       <c r="C24">
-        <v>4.31588495476718</v>
+        <v>-1.626334856703671</v>
       </c>
       <c r="D24">
-        <v>2.981849920083812</v>
+        <v>7.042899899225441</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -871,10 +871,10 @@
         <v>-6.189085285809249</v>
       </c>
       <c r="C25">
-        <v>-7.19655284112457</v>
+        <v>-9.28758839008329</v>
       </c>
       <c r="D25">
-        <v>-5.731044708871414</v>
+        <v>-2.567162040239357</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -885,10 +885,10 @@
         <v>-0.01004310457615176</v>
       </c>
       <c r="C26">
-        <v>-0.07298826753073806</v>
+        <v>-1.995882370427571</v>
       </c>
       <c r="D26">
-        <v>-0.1222832577716715</v>
+        <v>2.172343226982432</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -899,10 +899,10 @@
         <v>0.3634036878042313</v>
       </c>
       <c r="C27">
-        <v>0.1997182675727682</v>
+        <v>-2.457443688369687</v>
       </c>
       <c r="D27">
-        <v>-0.02873145913346864</v>
+        <v>3.511402829487098</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -913,10 +913,10 @@
         <v>-3.931257346331785</v>
       </c>
       <c r="C28">
-        <v>-5.191733529897546</v>
+        <v>-9.540190186306319</v>
       </c>
       <c r="D28">
-        <v>-2.551784652955225</v>
+        <v>1.851338375843281</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -927,10 +927,10 @@
         <v>-0.9223998484439555</v>
       </c>
       <c r="C29">
-        <v>-2.054483260968443</v>
+        <v>-5.703349166695681</v>
       </c>
       <c r="D29">
-        <v>-0.3044352724503652</v>
+        <v>3.434529998689184</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -941,10 +941,10 @@
         <v>-2.347511090212417</v>
       </c>
       <c r="C30">
-        <v>-3.674460529034018</v>
+        <v>-7.883192160846653</v>
       </c>
       <c r="D30">
-        <v>-1.02487994751127</v>
+        <v>3.391976355012405</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -955,10 +955,10 @@
         <v>2.743557709929778</v>
       </c>
       <c r="C31">
-        <v>3.00193553779593</v>
+        <v>-0.132097697872835</v>
       </c>
       <c r="D31">
-        <v>2.453023581936842</v>
+        <v>5.791697719361966</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -969,10 +969,10 @@
         <v>-1.314864717719244</v>
       </c>
       <c r="C32">
-        <v>-1.372409507570604</v>
+        <v>-3.655847344489593</v>
       </c>
       <c r="D32">
-        <v>-1.084107644834631</v>
+        <v>0.9938410023416999</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -983,10 +983,10 @@
         <v>4.953805491202434</v>
       </c>
       <c r="C33">
-        <v>4.857843623663904</v>
+        <v>1.900217324304676</v>
       </c>
       <c r="D33">
-        <v>4.775398992058921</v>
+        <v>7.994627897889983</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -997,10 +997,10 @@
         <v>0.9507545170562404</v>
       </c>
       <c r="C34">
-        <v>1.196343484373319</v>
+        <v>-2.061375672485499</v>
       </c>
       <c r="D34">
-        <v>1.19571227091626</v>
+        <v>3.801018057852512</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1011,10 +1011,10 @@
         <v>-3.915387946583038</v>
       </c>
       <c r="C35">
-        <v>-4.592681112324215</v>
+        <v>-6.472377563371811</v>
       </c>
       <c r="D35">
-        <v>-3.54614424371581</v>
+        <v>-1.362223302897791</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1025,10 +1025,10 @@
         <v>0.04146741636057438</v>
       </c>
       <c r="C36">
-        <v>0.1439102660367064</v>
+        <v>-3.42875879737371</v>
       </c>
       <c r="D36">
-        <v>0.1976084751432738</v>
+        <v>3.137309320630766</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1039,10 +1039,10 @@
         <v>0.6425517067009334</v>
       </c>
       <c r="C37">
-        <v>-0.03157049795804445</v>
+        <v>-2.991585692138232</v>
       </c>
       <c r="D37">
-        <v>0.5315992072280507</v>
+        <v>4.115610394396385</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1053,10 +1053,10 @@
         <v>-0.08465536927001471</v>
       </c>
       <c r="C38">
-        <v>-0.1047601685030153</v>
+        <v>-3.676000334441809</v>
       </c>
       <c r="D38">
-        <v>-0.1654661741528507</v>
+        <v>2.969678772021767</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1067,10 +1067,10 @@
         <v>-0.5429720961911744</v>
       </c>
       <c r="C39">
-        <v>-1.451579705737083</v>
+        <v>-5.06665337150568</v>
       </c>
       <c r="D39">
-        <v>0.523098257898913</v>
+        <v>3.949433207136255</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1081,10 +1081,10 @@
         <v>-5.665746083857637</v>
       </c>
       <c r="C40">
-        <v>-7.381706800723819</v>
+        <v>-10.8951310919454</v>
       </c>
       <c r="D40">
-        <v>-4.390047694138699</v>
+        <v>-0.3375281937973429</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1095,10 +1095,10 @@
         <v>3.79177473854091</v>
       </c>
       <c r="C41">
-        <v>4.58427852517973</v>
+        <v>0.6901253132752361</v>
       </c>
       <c r="D41">
-        <v>3.461105546529142</v>
+        <v>6.589542588563235</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1109,10 +1109,10 @@
         <v>0.7785433327984759</v>
       </c>
       <c r="C42">
-        <v>0.4608661379496226</v>
+        <v>-1.721483162111392</v>
       </c>
       <c r="D42">
-        <v>0.7530718242237944</v>
+        <v>4.101776676959679</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1123,10 +1123,10 @@
         <v>1.315437658403495</v>
       </c>
       <c r="C43">
-        <v>1.366545420768572</v>
+        <v>-1.294177313495837</v>
       </c>
       <c r="D43">
-        <v>1.679672769140805</v>
+        <v>4.051273380556597</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1137,10 +1137,10 @@
         <v>-1.614962083324634</v>
       </c>
       <c r="C44">
-        <v>-1.935264914729096</v>
+        <v>-4.323823421201311</v>
       </c>
       <c r="D44">
-        <v>-1.263274213996668</v>
+        <v>0.8249507386989263</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1151,10 +1151,10 @@
         <v>0.4675030422965465</v>
       </c>
       <c r="C45">
-        <v>0.2896957552140922</v>
+        <v>-4.7945702258127</v>
       </c>
       <c r="D45">
-        <v>1.096501119460047</v>
+        <v>4.664635848788401</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1165,10 +1165,10 @@
         <v>-0.2496453175728108</v>
       </c>
       <c r="C46">
-        <v>-0.4718878252810255</v>
+        <v>-2.683594819994117</v>
       </c>
       <c r="D46">
-        <v>-1.710331274025334</v>
+        <v>3.359661780826251</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1179,10 +1179,10 @@
         <v>2.578123769684448</v>
       </c>
       <c r="C47">
-        <v>3.145990400869803</v>
+        <v>-0.2157515231801521</v>
       </c>
       <c r="D47">
-        <v>2.715621358523457</v>
+        <v>4.836737369774324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>